<commit_message>
finish analysis of the final test
</commit_message>
<xml_diff>
--- a/Others/TestCuts/17TestCut2SeuilFunc1+addmipstart/pre_cut2_seuil_func_mipstart.xlsx
+++ b/Others/TestCuts/17TestCut2SeuilFunc1+addmipstart/pre_cut2_seuil_func_mipstart.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="pre_cut2_seuil_func_mipstart" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="opt" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="685">
   <si>
     <t>Sc(N/M)</t>
   </si>
@@ -2075,10 +2075,7 @@
     <t>max</t>
   </si>
   <si>
-    <t>without mipstart</t>
-  </si>
-  <si>
-    <t>去掉极值</t>
+    <t>seuil1_</t>
   </si>
 </sst>
 </file>
@@ -2598,7 +2595,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -2608,11 +2605,13 @@
     <xf numFmtId="0" fontId="14" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2936,8 +2935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O137"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104:E104"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N104" activeCellId="1" sqref="I50:I104 N50:N104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2989,7 +2988,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3036,7 +3035,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -3083,7 +3082,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -3130,7 +3129,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -3177,7 +3176,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -3224,7 +3223,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -3271,7 +3270,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -3318,7 +3317,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -3365,7 +3364,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -3412,7 +3411,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3459,7 +3458,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -3506,7 +3505,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -3553,7 +3552,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -3600,7 +3599,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -3647,7 +3646,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -3694,7 +3693,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -3741,7 +3740,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -3788,7 +3787,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -3835,7 +3834,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -3882,7 +3881,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -3929,7 +3928,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -3976,7 +3975,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -4023,7 +4022,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -4070,7 +4069,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -4117,7 +4116,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>94</v>
       </c>
@@ -4164,7 +4163,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -4211,7 +4210,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -4258,7 +4257,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>106</v>
       </c>
@@ -4305,7 +4304,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -4352,7 +4351,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -4399,7 +4398,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>118</v>
       </c>
@@ -4446,7 +4445,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>123</v>
       </c>
@@ -4493,7 +4492,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>128</v>
       </c>
@@ -4540,7 +4539,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>133</v>
       </c>
@@ -4587,7 +4586,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -4634,7 +4633,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -4681,7 +4680,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>149</v>
       </c>
@@ -4728,7 +4727,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>153</v>
       </c>
@@ -4775,7 +4774,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>157</v>
       </c>
@@ -4822,7 +4821,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>162</v>
       </c>
@@ -4869,7 +4868,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>167</v>
       </c>
@@ -4916,7 +4915,7 @@
         <v>1704</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>172</v>
       </c>
@@ -4963,7 +4962,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>176</v>
       </c>
@@ -5010,7 +5009,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>180</v>
       </c>
@@ -5057,7 +5056,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>183</v>
       </c>
@@ -5104,7 +5103,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>187</v>
       </c>
@@ -5151,7 +5150,7 @@
         <v>1512</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>192</v>
       </c>
@@ -5198,7 +5197,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>196</v>
       </c>
@@ -6210,7 +6209,7 @@
       <c r="H70">
         <v>1</v>
       </c>
-      <c r="I70" t="s">
+      <c r="I70" s="13" t="s">
         <v>303</v>
       </c>
       <c r="J70">
@@ -6257,7 +6256,7 @@
       <c r="H71">
         <v>1</v>
       </c>
-      <c r="I71" t="s">
+      <c r="I71" s="13" t="s">
         <v>306</v>
       </c>
       <c r="J71">
@@ -6304,7 +6303,7 @@
       <c r="H72">
         <v>1</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I72" s="12" t="s">
         <v>314</v>
       </c>
       <c r="J72">
@@ -6445,7 +6444,7 @@
       <c r="H75">
         <v>1</v>
       </c>
-      <c r="I75" t="s">
+      <c r="I75" s="13" t="s">
         <v>330</v>
       </c>
       <c r="J75">
@@ -6492,7 +6491,7 @@
       <c r="H76">
         <v>1</v>
       </c>
-      <c r="I76" t="s">
+      <c r="I76" s="13" t="s">
         <v>336</v>
       </c>
       <c r="J76">
@@ -6586,7 +6585,7 @@
       <c r="H78">
         <v>1</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I78" s="12" t="s">
         <v>347</v>
       </c>
       <c r="J78">
@@ -6680,7 +6679,7 @@
       <c r="H80">
         <v>1</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I80" s="12" t="s">
         <v>358</v>
       </c>
       <c r="J80">
@@ -6915,7 +6914,7 @@
       <c r="H85">
         <v>1</v>
       </c>
-      <c r="I85" t="s">
+      <c r="I85" s="13" t="s">
         <v>384</v>
       </c>
       <c r="J85">
@@ -7009,7 +7008,7 @@
       <c r="H87">
         <v>1</v>
       </c>
-      <c r="I87" t="s">
+      <c r="I87" s="12" t="s">
         <v>395</v>
       </c>
       <c r="J87">
@@ -7056,7 +7055,7 @@
       <c r="H88">
         <v>1</v>
       </c>
-      <c r="I88" t="s">
+      <c r="I88" s="12" t="s">
         <v>401</v>
       </c>
       <c r="J88">
@@ -7103,7 +7102,7 @@
       <c r="H89">
         <v>1</v>
       </c>
-      <c r="I89" t="s">
+      <c r="I89" s="13" t="s">
         <v>407</v>
       </c>
       <c r="J89">
@@ -7197,7 +7196,7 @@
       <c r="H91">
         <v>1</v>
       </c>
-      <c r="I91" t="s">
+      <c r="I91" s="13" t="s">
         <v>418</v>
       </c>
       <c r="J91">
@@ -7244,7 +7243,7 @@
       <c r="H92">
         <v>1</v>
       </c>
-      <c r="I92" t="s">
+      <c r="I92" s="12" t="s">
         <v>421</v>
       </c>
       <c r="J92">
@@ -7291,7 +7290,7 @@
       <c r="H93">
         <v>1</v>
       </c>
-      <c r="I93" t="s">
+      <c r="I93" s="12" t="s">
         <v>428</v>
       </c>
       <c r="J93">
@@ -7338,7 +7337,7 @@
       <c r="H94">
         <v>1</v>
       </c>
-      <c r="I94" t="s">
+      <c r="I94" s="13" t="s">
         <v>434</v>
       </c>
       <c r="J94">
@@ -7479,7 +7478,7 @@
       <c r="H97">
         <v>1</v>
       </c>
-      <c r="I97" t="s">
+      <c r="I97" s="12" t="s">
         <v>450</v>
       </c>
       <c r="J97">
@@ -7526,7 +7525,7 @@
       <c r="H98">
         <v>1</v>
       </c>
-      <c r="I98" t="s">
+      <c r="I98" s="12" t="s">
         <v>456</v>
       </c>
       <c r="J98">
@@ -7573,7 +7572,7 @@
       <c r="H99">
         <v>1</v>
       </c>
-      <c r="I99" t="s">
+      <c r="I99" s="13" t="s">
         <v>462</v>
       </c>
       <c r="J99">
@@ -7667,7 +7666,7 @@
       <c r="H101">
         <v>1</v>
       </c>
-      <c r="I101" t="s">
+      <c r="I101" s="13" t="s">
         <v>473</v>
       </c>
       <c r="J101">
@@ -7761,7 +7760,7 @@
       <c r="H103">
         <v>1</v>
       </c>
-      <c r="I103" t="s">
+      <c r="I103" s="13" t="s">
         <v>484</v>
       </c>
       <c r="J103">
@@ -9390,8 +9389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9923,11 +9922,9 @@
         <f t="shared" si="0"/>
         <v>8.1447963800905043</v>
       </c>
-      <c r="F35" s="9" t="s">
-        <v>684</v>
-      </c>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -9943,15 +9940,6 @@
         <f t="shared" si="0"/>
         <v>4.854368932038839</v>
       </c>
-      <c r="F36" t="s">
-        <v>681</v>
-      </c>
-      <c r="G36" t="s">
-        <v>682</v>
-      </c>
-      <c r="H36" t="s">
-        <v>683</v>
-      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -9967,15 +9955,6 @@
         <f t="shared" si="0"/>
         <v>-1.1627906976744196</v>
       </c>
-      <c r="F37">
-        <v>-37.86093786093786</v>
-      </c>
-      <c r="G37">
-        <v>-7.0947764826244493</v>
-      </c>
-      <c r="H37">
-        <v>9.4681085853012554</v>
-      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -9991,15 +9970,6 @@
         <f t="shared" si="0"/>
         <v>-16.176470588235308</v>
       </c>
-      <c r="F38">
-        <v>-33.349867724867714</v>
-      </c>
-      <c r="G38">
-        <v>-7.7487757597925695</v>
-      </c>
-      <c r="H38">
-        <v>22.205573868744395</v>
-      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -10014,15 +9984,6 @@
       <c r="D39" s="8">
         <f t="shared" si="0"/>
         <v>14.666666666666664</v>
-      </c>
-      <c r="F39">
-        <v>-49.772632693981009</v>
-      </c>
-      <c r="G39">
-        <v>-7.6446365458135492</v>
-      </c>
-      <c r="H39">
-        <v>51.320731482051599</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -11055,19 +11016,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H104"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="8"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11080,1617 +11043,645 @@
       <c r="D1" s="8" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2">
-        <v>0.08</v>
-      </c>
-      <c r="C2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D2" s="8">
-        <f>(C2-B2)/B2*100</f>
-        <v>75.000000000000014</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="9">
+        <v>129.87</v>
+      </c>
+      <c r="C2" s="9">
+        <v>111.6</v>
+      </c>
+      <c r="D2" s="10">
+        <f t="shared" ref="D2:D34" si="0">(C2-B2)/B2*100</f>
+        <v>-14.067914067914074</v>
+      </c>
+      <c r="E2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>0.08</v>
+        <v>205</v>
+      </c>
+      <c r="B3" s="2">
+        <v>526.49</v>
       </c>
       <c r="C3">
-        <v>0.19</v>
-      </c>
-      <c r="D3" s="8">
-        <f>(C3-B3)/B3*100</f>
-        <v>137.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>742.09</v>
+      </c>
+      <c r="D3" s="10">
+        <f t="shared" si="0"/>
+        <v>40.950445402571752</v>
+      </c>
+      <c r="E3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>0.06</v>
+        <v>210</v>
+      </c>
+      <c r="B4" s="2">
+        <v>90.62</v>
       </c>
       <c r="C4">
-        <v>0.05</v>
-      </c>
-      <c r="D4" s="8">
-        <f t="shared" ref="D4:D67" si="0">(C4-B4)/B4*100</f>
-        <v>-16.666666666666661</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90.18</v>
+      </c>
+      <c r="D4" s="10">
+        <f t="shared" si="0"/>
+        <v>-0.48554403001544666</v>
+      </c>
+      <c r="E4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>215</v>
       </c>
       <c r="B5">
-        <v>0.06</v>
+        <v>8.6</v>
       </c>
       <c r="C5">
-        <v>0.05</v>
-      </c>
-      <c r="D5" s="8">
+        <v>7.61</v>
+      </c>
+      <c r="D5" s="10">
         <f t="shared" si="0"/>
-        <v>-16.666666666666661</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-11.511627906976738</v>
+      </c>
+      <c r="E5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>220</v>
       </c>
       <c r="B6">
-        <v>0.08</v>
+        <v>7.18</v>
       </c>
       <c r="C6">
-        <v>0.09</v>
-      </c>
-      <c r="D6" s="8">
+        <v>6.46</v>
+      </c>
+      <c r="D6" s="10">
         <f t="shared" si="0"/>
-        <v>12.499999999999993</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-10.02785515320334</v>
+      </c>
+      <c r="E6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7">
-        <v>0.11</v>
+        <v>225</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1100.71</v>
       </c>
       <c r="C7">
-        <v>0.11</v>
-      </c>
-      <c r="D7" s="8">
+        <v>852.77</v>
+      </c>
+      <c r="D7" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-22.525460838913069</v>
+      </c>
+      <c r="E7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>230</v>
       </c>
       <c r="B8">
-        <v>0.08</v>
+        <v>6.63</v>
       </c>
       <c r="C8">
-        <v>0.09</v>
-      </c>
-      <c r="D8" s="8">
+        <v>6.29</v>
+      </c>
+      <c r="D8" s="10">
         <f t="shared" si="0"/>
-        <v>12.499999999999993</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-5.128205128205126</v>
+      </c>
+      <c r="E8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>235</v>
       </c>
       <c r="B9">
-        <v>0.09</v>
+        <v>3.67</v>
       </c>
       <c r="C9">
-        <v>0.11</v>
-      </c>
-      <c r="D9" s="8">
+        <v>3.99</v>
+      </c>
+      <c r="D9" s="10">
         <f t="shared" si="0"/>
-        <v>22.222222222222225</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8.7193460490463295</v>
+      </c>
+      <c r="E9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="B10">
-        <v>0.05</v>
+        <v>1.4</v>
       </c>
       <c r="C10">
-        <v>0.05</v>
-      </c>
-      <c r="D10" s="8">
+        <v>1.59</v>
+      </c>
+      <c r="D10" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13.571428571428584</v>
+      </c>
+      <c r="E10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11">
-        <v>0.05</v>
+        <v>244</v>
+      </c>
+      <c r="B11" s="2">
+        <v>112.07</v>
       </c>
       <c r="C11">
-        <v>0.06</v>
-      </c>
-      <c r="D11" s="8">
+        <v>76.989999999999995</v>
+      </c>
+      <c r="D11" s="10">
         <f t="shared" si="0"/>
-        <v>19.999999999999989</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-31.301864905862409</v>
+      </c>
+      <c r="E11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>249</v>
       </c>
       <c r="B12">
-        <v>0.05</v>
+        <v>13.23</v>
       </c>
       <c r="C12">
-        <v>0.03</v>
-      </c>
-      <c r="D12" s="8">
+        <v>10.65</v>
+      </c>
+      <c r="D12" s="10">
         <f t="shared" si="0"/>
-        <v>-40.000000000000007</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-19.501133786848072</v>
+      </c>
+      <c r="E12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>254</v>
       </c>
       <c r="B13">
-        <v>0.11</v>
+        <v>18.45</v>
       </c>
       <c r="C13">
-        <v>0.11</v>
-      </c>
-      <c r="D13" s="8">
+        <v>26.63</v>
+      </c>
+      <c r="D13" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44.3360433604336</v>
+      </c>
+      <c r="E13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>259</v>
       </c>
       <c r="B14">
-        <v>0.05</v>
+        <v>28.7</v>
       </c>
       <c r="C14">
-        <v>0.05</v>
-      </c>
-      <c r="D14" s="8">
+        <v>28.67</v>
+      </c>
+      <c r="D14" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-0.10452961672473027</v>
+      </c>
+      <c r="E14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>264</v>
       </c>
       <c r="B15">
-        <v>0.05</v>
+        <v>12.65</v>
       </c>
       <c r="C15">
-        <v>0.05</v>
-      </c>
-      <c r="D15" s="8">
+        <v>8.83</v>
+      </c>
+      <c r="D15" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-30.197628458498027</v>
+      </c>
+      <c r="E15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>269</v>
       </c>
       <c r="B16">
-        <v>0.05</v>
+        <v>6.94</v>
       </c>
       <c r="C16">
-        <v>0.05</v>
-      </c>
-      <c r="D16" s="8">
+        <v>7.32</v>
+      </c>
+      <c r="D16" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.475504322766569</v>
+      </c>
+      <c r="E16" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>274</v>
       </c>
       <c r="B17">
-        <v>0.08</v>
+        <v>17.41</v>
       </c>
       <c r="C17">
-        <v>0.11</v>
-      </c>
-      <c r="D17" s="8">
+        <v>16.32</v>
+      </c>
+      <c r="D17" s="10">
         <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-6.2607696726019526</v>
+      </c>
+      <c r="E17" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18">
-        <v>0.06</v>
+        <v>279</v>
+      </c>
+      <c r="B18" s="2">
+        <v>135.86000000000001</v>
       </c>
       <c r="C18">
-        <v>0.06</v>
-      </c>
-      <c r="D18" s="8">
+        <v>59.95</v>
+      </c>
+      <c r="D18" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-55.873693508022967</v>
+      </c>
+      <c r="E18" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>284</v>
       </c>
       <c r="B19">
-        <v>0.01</v>
+        <v>14.4</v>
       </c>
       <c r="C19">
-        <v>0.01</v>
-      </c>
-      <c r="D19" s="8">
+        <v>13.87</v>
+      </c>
+      <c r="D19" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-3.6805555555555634</v>
+      </c>
+      <c r="E19" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20">
-        <v>0.31</v>
+        <v>289</v>
+      </c>
+      <c r="B20" s="4">
+        <v>10.58</v>
       </c>
       <c r="C20">
-        <v>0.33</v>
-      </c>
-      <c r="D20" s="8">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="D20" s="10">
         <f t="shared" si="0"/>
-        <v>6.4516129032258114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-8.9792060491493313</v>
+      </c>
+      <c r="E20" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>294</v>
       </c>
       <c r="B21">
-        <v>0.61</v>
+        <v>8.2100000000000009</v>
       </c>
       <c r="C21">
-        <v>0.53</v>
-      </c>
-      <c r="D21" s="8">
+        <v>6.47</v>
+      </c>
+      <c r="D21" s="10">
         <f t="shared" si="0"/>
-        <v>-13.114754098360649</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-21.193666260657746</v>
+      </c>
+      <c r="E21" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="C22">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="D22" s="8">
+        <v>316</v>
+      </c>
+      <c r="B22" s="2">
+        <v>99.37</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1802.33</v>
+      </c>
+      <c r="D22" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1713.7566670021133</v>
+      </c>
+      <c r="E22" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23">
-        <v>0.2</v>
+        <v>321</v>
+      </c>
+      <c r="B23" s="2">
+        <v>60.48</v>
       </c>
       <c r="C23">
-        <v>0.22</v>
-      </c>
-      <c r="D23" s="8">
+        <v>1802.19</v>
+      </c>
+      <c r="D23" s="10">
         <f t="shared" si="0"/>
-        <v>9.9999999999999947</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2879.8115079365084</v>
+      </c>
+      <c r="E23" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24">
-        <v>0.64</v>
+        <v>338</v>
+      </c>
+      <c r="B24" s="5">
+        <v>536.09</v>
       </c>
       <c r="C24">
-        <v>0.66</v>
-      </c>
-      <c r="D24" s="8">
+        <v>1445.65</v>
+      </c>
+      <c r="D24" s="10">
         <f t="shared" si="0"/>
-        <v>3.1250000000000027</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>169.66554123374806</v>
+      </c>
+      <c r="E24" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>90</v>
-      </c>
-      <c r="B25">
-        <v>0.25</v>
+        <v>360</v>
+      </c>
+      <c r="B25" s="6">
+        <v>788.49</v>
       </c>
       <c r="C25">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="D25" s="8">
+        <v>108.78</v>
+      </c>
+      <c r="D25" s="10">
         <f t="shared" si="0"/>
-        <v>12.000000000000011</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-86.204010196705099</v>
+      </c>
+      <c r="E25" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26">
-        <v>0.81</v>
+        <v>365</v>
+      </c>
+      <c r="B26" s="2">
+        <v>95.94</v>
       </c>
       <c r="C26">
-        <v>0.83</v>
-      </c>
-      <c r="D26" s="8">
+        <v>25.57</v>
+      </c>
+      <c r="D26" s="10">
         <f t="shared" si="0"/>
-        <v>2.4691358024691241</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-73.347925786950185</v>
+      </c>
+      <c r="E26" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27">
-        <v>0.28999999999999998</v>
+        <v>375</v>
+      </c>
+      <c r="B27" s="2">
+        <v>266.2</v>
       </c>
       <c r="C27">
-        <v>0.34</v>
-      </c>
-      <c r="D27" s="8">
+        <v>1803.49</v>
+      </c>
+      <c r="D27" s="10">
         <f t="shared" si="0"/>
-        <v>17.241379310344847</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>577.49436513899332</v>
+      </c>
+      <c r="E27" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28">
-        <v>0.23</v>
+        <v>386</v>
+      </c>
+      <c r="B28" s="2">
+        <v>266.95999999999998</v>
       </c>
       <c r="C28">
-        <v>0.27</v>
-      </c>
-      <c r="D28" s="8">
+        <v>1801.55</v>
+      </c>
+      <c r="D28" s="10">
         <f t="shared" si="0"/>
-        <v>17.39130434782609</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>574.8389271801019</v>
+      </c>
+      <c r="E28" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>106</v>
-      </c>
-      <c r="B29">
-        <v>0.25</v>
+        <v>409</v>
+      </c>
+      <c r="B29" s="2">
+        <v>172.85</v>
       </c>
       <c r="C29">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="D29" s="8">
+        <v>522.29</v>
+      </c>
+      <c r="D29" s="10">
         <f t="shared" si="0"/>
-        <v>12.000000000000011</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>202.16372577379227</v>
+      </c>
+      <c r="E29" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>110</v>
-      </c>
-      <c r="B30">
-        <v>0.2</v>
+        <v>436</v>
+      </c>
+      <c r="B30" s="2">
+        <v>358.5</v>
       </c>
       <c r="C30">
-        <v>0.23</v>
-      </c>
-      <c r="D30" s="8">
+        <v>1087.28</v>
+      </c>
+      <c r="D30" s="10">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>203.28591352859132</v>
+      </c>
+      <c r="E30" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>114</v>
-      </c>
-      <c r="B31">
-        <v>1.84</v>
+        <v>441</v>
+      </c>
+      <c r="B31" s="2">
+        <v>162.41</v>
       </c>
       <c r="C31">
-        <v>1.73</v>
-      </c>
-      <c r="D31" s="8">
+        <v>1124.29</v>
+      </c>
+      <c r="D31" s="10">
         <f t="shared" si="0"/>
-        <v>-5.9782608695652222</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>592.25417154116121</v>
+      </c>
+      <c r="E31" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>464</v>
       </c>
       <c r="B32">
-        <v>1.72</v>
+        <v>1321.65</v>
       </c>
       <c r="C32">
-        <v>1.86</v>
-      </c>
-      <c r="D32" s="8">
+        <v>1236.96</v>
+      </c>
+      <c r="D32" s="10">
         <f t="shared" si="0"/>
-        <v>8.1395348837209376</v>
+        <v>-6.4078992168879845</v>
+      </c>
+      <c r="E32" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>123</v>
-      </c>
-      <c r="B33">
-        <v>1.92</v>
+        <v>475</v>
+      </c>
+      <c r="B33" s="2">
+        <v>346.06</v>
       </c>
       <c r="C33">
-        <v>1.87</v>
-      </c>
-      <c r="D33" s="8">
+        <v>708.87</v>
+      </c>
+      <c r="D33" s="10">
         <f t="shared" si="0"/>
-        <v>-2.6041666666666572</v>
+        <v>104.84020112119285</v>
+      </c>
+      <c r="E33" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>128</v>
-      </c>
-      <c r="B34">
-        <v>0.97</v>
+        <v>486</v>
+      </c>
+      <c r="B34" s="2">
+        <v>273.08</v>
       </c>
       <c r="C34">
-        <v>1.06</v>
-      </c>
-      <c r="D34" s="8">
+        <v>80.680000000000007</v>
+      </c>
+      <c r="D34" s="10">
         <f t="shared" si="0"/>
-        <v>9.2783505154639254</v>
+        <v>-70.45554416288266</v>
+      </c>
+      <c r="E34" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>133</v>
-      </c>
-      <c r="B35">
-        <v>2.21</v>
-      </c>
-      <c r="C35">
-        <v>2.39</v>
-      </c>
-      <c r="D35" s="8">
-        <f t="shared" si="0"/>
-        <v>8.1447963800905043</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>684</v>
-      </c>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>138</v>
-      </c>
-      <c r="B36">
-        <v>1.03</v>
-      </c>
-      <c r="C36">
-        <v>1.08</v>
-      </c>
-      <c r="D36" s="8">
-        <f t="shared" si="0"/>
-        <v>4.854368932038839</v>
-      </c>
-      <c r="F36" t="s">
-        <v>681</v>
-      </c>
-      <c r="G36" t="s">
-        <v>682</v>
-      </c>
-      <c r="H36" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>144</v>
-      </c>
-      <c r="B37">
-        <v>1.72</v>
-      </c>
-      <c r="C37">
-        <v>1.7</v>
-      </c>
-      <c r="D37" s="8">
-        <f t="shared" si="0"/>
-        <v>-1.1627906976744196</v>
-      </c>
-      <c r="F37">
-        <v>-37.86093786093786</v>
-      </c>
-      <c r="G37">
-        <v>-7.0947764826244493</v>
-      </c>
-      <c r="H37">
-        <v>9.4681085853012554</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>149</v>
-      </c>
-      <c r="B38">
-        <v>1.36</v>
-      </c>
-      <c r="C38">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="D38" s="8">
-        <f t="shared" si="0"/>
-        <v>-16.176470588235308</v>
-      </c>
-      <c r="F38">
-        <v>-33.349867724867714</v>
-      </c>
-      <c r="G38">
-        <v>-7.7487757597925695</v>
-      </c>
-      <c r="H38">
-        <v>22.205573868744395</v>
-      </c>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>153</v>
-      </c>
-      <c r="B39">
-        <v>0.75</v>
-      </c>
-      <c r="C39">
-        <v>0.86</v>
-      </c>
-      <c r="D39" s="8">
-        <f t="shared" si="0"/>
-        <v>14.666666666666664</v>
-      </c>
-      <c r="F39">
-        <v>-49.772632693981009</v>
-      </c>
-      <c r="G39">
-        <v>-7.6446365458135492</v>
-      </c>
-      <c r="H39">
-        <v>51.320731482051599</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>157</v>
-      </c>
-      <c r="B40">
-        <v>1.21</v>
-      </c>
-      <c r="C40">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="D40" s="8">
-        <f t="shared" si="0"/>
-        <v>-7.4380165289256093</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>162</v>
-      </c>
-      <c r="B41">
-        <v>2.23</v>
-      </c>
-      <c r="C41">
-        <v>2.46</v>
-      </c>
-      <c r="D41" s="8">
-        <f t="shared" si="0"/>
-        <v>10.313901345291479</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>167</v>
-      </c>
-      <c r="B42">
-        <v>2.56</v>
-      </c>
-      <c r="C42">
-        <v>2.36</v>
-      </c>
-      <c r="D42" s="8">
-        <f t="shared" si="0"/>
-        <v>-7.8125000000000071</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>172</v>
-      </c>
-      <c r="B43">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="C43">
-        <v>1.81</v>
-      </c>
-      <c r="D43" s="8">
-        <f t="shared" si="0"/>
-        <v>-25.514403292181072</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>176</v>
-      </c>
-      <c r="B44">
-        <v>1.33</v>
-      </c>
-      <c r="C44">
-        <v>1.25</v>
-      </c>
-      <c r="D44" s="8">
-        <f t="shared" si="0"/>
-        <v>-6.0150375939849674</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>180</v>
-      </c>
-      <c r="B45">
-        <v>0.83</v>
-      </c>
-      <c r="C45">
-        <v>0.83</v>
-      </c>
-      <c r="D45" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>183</v>
-      </c>
-      <c r="B46">
-        <v>27.94</v>
-      </c>
-      <c r="C46">
-        <v>26.74</v>
-      </c>
-      <c r="D46" s="8">
-        <f t="shared" si="0"/>
-        <v>-4.2949176807444625</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>187</v>
-      </c>
-      <c r="B47">
-        <v>2.39</v>
-      </c>
-      <c r="C47">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="D47" s="8">
-        <f t="shared" si="0"/>
-        <v>-15.062761506276162</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>192</v>
-      </c>
-      <c r="B48">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="C48">
-        <v>1.28</v>
-      </c>
-      <c r="D48" s="8">
-        <f t="shared" si="0"/>
-        <v>17.431192660550451</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>196</v>
-      </c>
-      <c r="B49">
-        <v>0.97</v>
-      </c>
-      <c r="C49">
-        <v>1.04</v>
-      </c>
-      <c r="D49" s="8">
-        <f t="shared" si="0"/>
-        <v>7.2164948453608311</v>
-      </c>
-      <c r="F49" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="B50" s="10">
-        <v>129.87</v>
-      </c>
-      <c r="C50" s="10">
-        <v>111.6</v>
-      </c>
-      <c r="D50" s="11">
-        <f t="shared" si="0"/>
-        <v>-14.067914067914074</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>681</v>
-      </c>
-      <c r="G50" s="10" t="s">
-        <v>682</v>
-      </c>
-      <c r="H50" s="10" t="s">
-        <v>683</v>
-      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="10"/>
+    </row>
+    <row r="50" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50"/>
+      <c r="B50"/>
+      <c r="C50"/>
+      <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>205</v>
-      </c>
-      <c r="B51" s="2">
-        <v>526.49</v>
-      </c>
-      <c r="C51">
-        <v>742.09</v>
-      </c>
-      <c r="D51" s="8">
-        <f t="shared" si="0"/>
-        <v>40.950445402571752</v>
-      </c>
-      <c r="F51" s="8">
-        <f>MIN(D50:D69)</f>
-        <v>-31.301864905862409</v>
-      </c>
-      <c r="G51" s="8">
-        <f>AVERAGE(D50:D69)</f>
-        <v>-6.4582909491840219</v>
-      </c>
-      <c r="H51" s="8">
-        <f>MAX(D50:D69)</f>
-        <v>40.950445402571752</v>
-      </c>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>210</v>
-      </c>
-      <c r="B52" s="2">
-        <v>90.62</v>
-      </c>
-      <c r="C52">
-        <v>90.18</v>
-      </c>
-      <c r="D52" s="8">
-        <f t="shared" si="0"/>
-        <v>-0.48554403001544666</v>
-      </c>
-      <c r="F52" s="8">
-        <f>MIN(D70:D86)</f>
-        <v>-43.892105321532355</v>
-      </c>
-      <c r="G52" s="8">
-        <f>AVERAGE(D70:D86)</f>
-        <v>-10.490478219103426</v>
-      </c>
-      <c r="H52" s="8">
-        <f>MAX(D70:D86)</f>
-        <v>9.4696588507597816</v>
-      </c>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>215</v>
-      </c>
-      <c r="B53">
-        <v>8.6</v>
-      </c>
-      <c r="C53">
-        <v>7.61</v>
-      </c>
-      <c r="D53" s="8">
-        <f t="shared" si="0"/>
-        <v>-11.511627906976738</v>
-      </c>
-      <c r="F53" s="8">
-        <f>MIN(D87:D104)</f>
-        <v>-48.276496339624032</v>
-      </c>
-      <c r="G53" s="8">
-        <f>AVERAGE(D87:D104)</f>
-        <v>-0.79031941658978178</v>
-      </c>
-      <c r="H53" s="8">
-        <f>MAX(D87:D104)</f>
-        <v>76.304426684140935</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>220</v>
-      </c>
-      <c r="B54">
-        <v>7.18</v>
-      </c>
-      <c r="C54">
-        <v>6.46</v>
-      </c>
-      <c r="D54" s="8">
-        <f t="shared" si="0"/>
-        <v>-10.02785515320334</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>225</v>
-      </c>
-      <c r="B55" s="3">
-        <v>1100.71</v>
-      </c>
-      <c r="C55">
-        <v>852.77</v>
-      </c>
-      <c r="D55" s="8">
-        <f t="shared" si="0"/>
-        <v>-22.525460838913069</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>230</v>
-      </c>
-      <c r="B56">
-        <v>6.63</v>
-      </c>
-      <c r="C56">
-        <v>6.29</v>
-      </c>
-      <c r="D56" s="8">
-        <f t="shared" si="0"/>
-        <v>-5.128205128205126</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>235</v>
-      </c>
-      <c r="B57">
-        <v>3.67</v>
-      </c>
-      <c r="C57">
-        <v>3.99</v>
-      </c>
-      <c r="D57" s="8">
-        <f t="shared" si="0"/>
-        <v>8.7193460490463295</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>240</v>
-      </c>
-      <c r="B58">
-        <v>1.4</v>
-      </c>
-      <c r="C58">
-        <v>1.59</v>
-      </c>
-      <c r="D58" s="8">
-        <f t="shared" si="0"/>
-        <v>13.571428571428584</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>244</v>
-      </c>
-      <c r="B59" s="2">
-        <v>112.07</v>
-      </c>
-      <c r="C59">
-        <v>76.989999999999995</v>
-      </c>
-      <c r="D59" s="8">
-        <f t="shared" si="0"/>
-        <v>-31.301864905862409</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>249</v>
-      </c>
-      <c r="B60">
-        <v>13.23</v>
-      </c>
-      <c r="C60">
-        <v>10.65</v>
-      </c>
-      <c r="D60" s="8">
-        <f t="shared" si="0"/>
-        <v>-19.501133786848072</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>254</v>
-      </c>
-      <c r="B61">
-        <v>18.45</v>
-      </c>
-      <c r="C61">
-        <v>26.63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>259</v>
-      </c>
-      <c r="B62">
-        <v>28.7</v>
-      </c>
-      <c r="C62">
-        <v>28.67</v>
-      </c>
-      <c r="D62" s="8">
-        <f t="shared" si="0"/>
-        <v>-0.10452961672473027</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>264</v>
-      </c>
-      <c r="B63">
-        <v>12.65</v>
-      </c>
-      <c r="C63">
-        <v>8.83</v>
-      </c>
-      <c r="D63" s="8">
-        <f t="shared" si="0"/>
-        <v>-30.197628458498027</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>269</v>
-      </c>
-      <c r="B64">
-        <v>6.94</v>
-      </c>
-      <c r="C64">
-        <v>7.32</v>
-      </c>
-      <c r="D64" s="8">
-        <f t="shared" si="0"/>
-        <v>5.475504322766569</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>274</v>
-      </c>
-      <c r="B65">
-        <v>17.41</v>
-      </c>
-      <c r="C65">
-        <v>16.32</v>
-      </c>
-      <c r="D65" s="8">
-        <f t="shared" si="0"/>
-        <v>-6.2607696726019526</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>279</v>
-      </c>
-      <c r="B66" s="2">
-        <v>135.86000000000001</v>
-      </c>
-      <c r="C66">
-        <v>59.95</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>284</v>
-      </c>
-      <c r="B67">
-        <v>14.4</v>
-      </c>
-      <c r="C67">
-        <v>13.87</v>
-      </c>
-      <c r="D67" s="8">
-        <f t="shared" si="0"/>
-        <v>-3.6805555555555634</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>289</v>
-      </c>
-      <c r="B68" s="4">
-        <v>10.58</v>
-      </c>
-      <c r="C68">
-        <v>9.6300000000000008</v>
-      </c>
-      <c r="D68" s="8">
-        <f t="shared" ref="D68:D104" si="1">(C68-B68)/B68*100</f>
-        <v>-8.9792060491493313</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>294</v>
-      </c>
-      <c r="B69">
-        <v>8.2100000000000009</v>
-      </c>
-      <c r="C69">
-        <v>6.47</v>
-      </c>
-      <c r="D69" s="8">
-        <f t="shared" si="1"/>
-        <v>-21.193666260657746</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="B70" s="10">
-        <v>1806.19</v>
-      </c>
-      <c r="C70" s="10">
-        <v>1802.33</v>
-      </c>
-      <c r="D70" s="11">
-        <f t="shared" si="1"/>
-        <v>-0.21370952114673028</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>305</v>
-      </c>
-      <c r="B71">
-        <v>1811.32</v>
-      </c>
-      <c r="C71">
-        <v>1802.19</v>
-      </c>
-      <c r="D71" s="8">
-        <f t="shared" si="1"/>
-        <v>-0.5040522933551157</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>310</v>
-      </c>
-      <c r="B72">
-        <v>1808</v>
-      </c>
-      <c r="C72">
-        <v>1445.65</v>
-      </c>
-      <c r="D72" s="8">
-        <f t="shared" si="1"/>
-        <v>-20.041482300884951</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>316</v>
-      </c>
-      <c r="B73" s="2">
-        <v>99.37</v>
-      </c>
-      <c r="C73">
-        <v>108.78</v>
-      </c>
-      <c r="D73" s="8">
-        <f t="shared" si="1"/>
-        <v>9.4696588507597816</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>321</v>
-      </c>
-      <c r="B74" s="2">
-        <v>60.48</v>
-      </c>
-      <c r="C74">
-        <v>25.57</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>326</v>
-      </c>
-      <c r="B75">
-        <v>1804.2</v>
-      </c>
-      <c r="C75">
-        <v>1803.49</v>
-      </c>
-      <c r="D75" s="8">
-        <f t="shared" si="1"/>
-        <v>-3.9352621660571796E-2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>332</v>
-      </c>
-      <c r="B76">
-        <v>1807.53</v>
-      </c>
-      <c r="C76">
-        <v>1801.55</v>
-      </c>
-      <c r="D76" s="8">
-        <f t="shared" si="1"/>
-        <v>-0.33083821568660099</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>338</v>
-      </c>
-      <c r="B77" s="5">
-        <v>536.09</v>
-      </c>
-      <c r="C77">
-        <v>522.29</v>
-      </c>
-      <c r="D77" s="8">
-        <f t="shared" si="1"/>
-        <v>-2.5741946314984552</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>343</v>
-      </c>
-      <c r="B78">
-        <v>1216.71</v>
-      </c>
-      <c r="C78">
-        <v>1087.28</v>
-      </c>
-      <c r="D78" s="8">
-        <f t="shared" si="1"/>
-        <v>-10.637703314676468</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>349</v>
-      </c>
-      <c r="B79" s="5">
-        <v>646.26</v>
-      </c>
-      <c r="C79">
-        <v>1124.29</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>354</v>
-      </c>
-      <c r="B80">
-        <v>1804.02</v>
-      </c>
-      <c r="C80">
-        <v>1236.96</v>
-      </c>
-      <c r="D80" s="8">
-        <f t="shared" si="1"/>
-        <v>-31.433132670369506</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>360</v>
-      </c>
-      <c r="B81" s="6">
-        <v>788.49</v>
-      </c>
-      <c r="C81">
-        <v>708.87</v>
-      </c>
-      <c r="D81" s="8">
-        <f t="shared" si="1"/>
-        <v>-10.097781836167865</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>365</v>
-      </c>
-      <c r="B82" s="2">
-        <v>95.94</v>
-      </c>
-      <c r="C82">
-        <v>80.680000000000007</v>
-      </c>
-      <c r="D82" s="8">
-        <f t="shared" si="1"/>
-        <v>-15.9057744423598</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>370</v>
-      </c>
-      <c r="B83">
-        <v>1803.24</v>
-      </c>
-      <c r="C83">
-        <v>1011.76</v>
-      </c>
-      <c r="D83" s="8">
-        <f t="shared" si="1"/>
-        <v>-43.892105321532355</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>375</v>
-      </c>
-      <c r="B84" s="2">
-        <v>266.2</v>
-      </c>
-      <c r="C84">
-        <v>200.68</v>
-      </c>
-      <c r="D84" s="8">
-        <f t="shared" si="1"/>
-        <v>-24.613072877535682</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>380</v>
-      </c>
-      <c r="B85">
-        <v>1809.03</v>
-      </c>
-      <c r="C85">
-        <v>1802.6</v>
-      </c>
-      <c r="D85" s="8">
-        <f t="shared" si="1"/>
-        <v>-0.35543910272356255</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>386</v>
-      </c>
-      <c r="B86" s="2">
-        <v>266.95999999999998</v>
-      </c>
-      <c r="C86">
-        <v>250.44</v>
-      </c>
-      <c r="D86" s="8">
-        <f t="shared" si="1"/>
-        <v>-6.1881929877135091</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="10" t="s">
-        <v>391</v>
-      </c>
-      <c r="B87" s="10">
-        <v>635.05999999999995</v>
-      </c>
-      <c r="C87" s="10">
-        <v>1522.13</v>
-      </c>
-      <c r="D87" s="11"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>397</v>
-      </c>
-      <c r="B88">
-        <v>1458.81</v>
-      </c>
-      <c r="C88">
-        <v>1730.4</v>
-      </c>
-      <c r="D88" s="8">
-        <f t="shared" si="1"/>
-        <v>18.617229111399027</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>403</v>
-      </c>
-      <c r="B89">
-        <v>1808.68</v>
-      </c>
-      <c r="C89">
-        <v>1809.59</v>
-      </c>
-      <c r="D89" s="8">
-        <f t="shared" si="1"/>
-        <v>5.0312935400394457E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>409</v>
-      </c>
-      <c r="B90" s="2">
-        <v>172.85</v>
-      </c>
-      <c r="C90">
-        <v>192.19</v>
-      </c>
-      <c r="D90" s="8">
-        <f t="shared" si="1"/>
-        <v>11.188892102979464</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>414</v>
-      </c>
-      <c r="B91">
-        <v>1804.97</v>
-      </c>
-      <c r="C91">
-        <v>1803.5</v>
-      </c>
-      <c r="D91" s="8">
-        <f t="shared" si="1"/>
-        <v>-8.1441796816569101E-2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>420</v>
-      </c>
-      <c r="B92" s="7">
-        <v>854.59</v>
-      </c>
-      <c r="C92">
-        <v>1506.68</v>
-      </c>
-      <c r="D92" s="8">
-        <f t="shared" si="1"/>
-        <v>76.304426684140935</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>424</v>
-      </c>
-      <c r="B93">
-        <v>1241.6500000000001</v>
-      </c>
-      <c r="C93">
-        <v>1527.91</v>
-      </c>
-      <c r="D93" s="8">
-        <f t="shared" si="1"/>
-        <v>23.054806104779928</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>430</v>
-      </c>
-      <c r="B94">
-        <v>1396</v>
-      </c>
-      <c r="C94">
-        <v>1804.35</v>
-      </c>
-      <c r="D94" s="8">
-        <f t="shared" si="1"/>
-        <v>29.25143266475644</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>436</v>
-      </c>
-      <c r="B95" s="2">
-        <v>358.5</v>
-      </c>
-      <c r="C95">
-        <v>226.89</v>
-      </c>
-      <c r="D95" s="8">
-        <f t="shared" si="1"/>
-        <v>-36.711297071129714</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>441</v>
-      </c>
-      <c r="B96" s="2">
-        <v>162.41</v>
-      </c>
-      <c r="C96">
-        <v>169.42</v>
-      </c>
-      <c r="D96" s="8">
-        <f t="shared" si="1"/>
-        <v>4.3162366849331884</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>446</v>
-      </c>
-      <c r="B97">
-        <v>1813.04</v>
-      </c>
-      <c r="C97">
-        <v>1554.45</v>
-      </c>
-      <c r="D97" s="8">
-        <f t="shared" si="1"/>
-        <v>-14.262785156422359</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>452</v>
-      </c>
-      <c r="B98">
-        <v>1630.98</v>
-      </c>
-      <c r="C98">
-        <v>843.6</v>
-      </c>
-      <c r="D98" s="8">
-        <f>(C98-B98)/B98*100</f>
-        <v>-48.276496339624032</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>458</v>
-      </c>
-      <c r="B99">
-        <v>1809.76</v>
-      </c>
-      <c r="C99">
-        <v>1808.32</v>
-      </c>
-      <c r="D99" s="8">
-        <f t="shared" si="1"/>
-        <v>-7.9568561577228733E-2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>464</v>
-      </c>
-      <c r="B100">
-        <v>1321.65</v>
-      </c>
-      <c r="C100">
-        <v>827.74</v>
-      </c>
-      <c r="D100" s="8">
-        <f t="shared" si="1"/>
-        <v>-37.370710853856927</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>469</v>
-      </c>
-      <c r="B101">
-        <v>1804.7</v>
-      </c>
-      <c r="C101">
-        <v>1803.61</v>
-      </c>
-      <c r="D101" s="8">
-        <f t="shared" si="1"/>
-        <v>-6.0397850058189477E-2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>475</v>
-      </c>
-      <c r="B102" s="2">
-        <v>346.06</v>
-      </c>
-      <c r="C102">
-        <v>212.58</v>
-      </c>
-      <c r="D102" s="8">
-        <f t="shared" si="1"/>
-        <v>-38.571346009362536</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>480</v>
-      </c>
-      <c r="B103">
-        <v>1805.14</v>
-      </c>
-      <c r="C103">
-        <v>1804.88</v>
-      </c>
-      <c r="D103" s="8">
-        <f t="shared" si="1"/>
-        <v>-1.4403314978339127E-2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>486</v>
-      </c>
-      <c r="B104" s="2">
-        <v>273.08</v>
-      </c>
-      <c r="C104">
-        <v>101.76</v>
-      </c>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+    </row>
+    <row r="70" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70"/>
+      <c r="B70"/>
+      <c r="C70"/>
+      <c r="D70" s="8"/>
+    </row>
+    <row r="87" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87"/>
+      <c r="B87"/>
+      <c r="C87"/>
+      <c r="D87" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>